<commit_message>
Added mean and variance values to raw data excel file. Updated arduino code, need to test
</commit_message>
<xml_diff>
--- a/project_3/t580_project_data.xlsx
+++ b/project_3/t580_project_data.xlsx
@@ -5,16 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merc.MERCURY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merc.MERCURY\Documents\ComputingandControl\project_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0F3CB2E-7D4E-4A3D-A85A-DC1C721F04FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{004119FF-7DA8-462E-88C6-739F2E22B4AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7098" windowHeight="2754" xr2:uid="{A6EF06F1-54AE-4E92-BB14-E64AC4F16E5A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7095" windowHeight="2760" xr2:uid="{A6EF06F1-54AE-4E92-BB14-E64AC4F16E5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">(Sheet1!$C$10,Sheet1!$C$10:$C$12,Sheet1!$C$23:$C$25,Sheet1!$C$36:$C$38)</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">(Sheet1!$C$13:$C$15,Sheet1!$C$26:$C$28,Sheet1!$C$39:$C$41)</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">(Sheet1!$C$32,Sheet1!$C$30:$C$32,Sheet1!$C$17:$C$19,Sheet1!$C$4:$C$6)</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">(Sheet1!$C$4,Sheet1!$C$4:$C$11,Sheet1!$C$12:$C$15,Sheet1!$C$17:$C$28,Sheet1!$C$30:$C$41)</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">(Sheet1!$C$7:$C$9,Sheet1!$C$20:$C$22,Sheet1!$C$33:$C$35)</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">(Sheet1!$C$10,Sheet1!$C$10:$C$12,Sheet1!$C$23:$C$25,Sheet1!$C$36:$C$38)</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">(Sheet1!$C$13:$C$15,Sheet1!$C$26:$C$28,Sheet1!$C$39:$C$41)</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">(Sheet1!$C$32,Sheet1!$C$30:$C$32,Sheet1!$C$17:$C$19,Sheet1!$C$4:$C$6)</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">(Sheet1!$C$4,Sheet1!$C$4:$C$11,Sheet1!$C$12:$C$15,Sheet1!$C$17:$C$28,Sheet1!$C$30:$C$41)</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">(Sheet1!$C$7:$C$9,Sheet1!$C$20:$C$22,Sheet1!$C$33:$C$35)</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
   <si>
     <t>Sensor1</t>
   </si>
@@ -58,6 +70,15 @@
   </si>
   <si>
     <t>Time Position on Oscilloscope (ms)</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Data between 3 sensors</t>
+  </si>
+  <si>
+    <t>Variance</t>
   </si>
 </sst>
 </file>
@@ -409,26 +430,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A5CB94-29D9-41D4-A28D-11E7E1479EBC}">
-  <dimension ref="A2:D41"/>
+  <dimension ref="A2:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83984375" customWidth="1"/>
-    <col min="2" max="2" width="20.26171875" customWidth="1"/>
-    <col min="3" max="3" width="34.5234375" customWidth="1"/>
-    <col min="4" max="4" width="31.7890625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -442,9 +465,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
       </c>
       <c r="B4">
         <v>868</v>
@@ -457,9 +480,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>2</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
       </c>
       <c r="B5">
         <v>900</v>
@@ -472,9 +495,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>2</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
       </c>
       <c r="B6">
         <v>900</v>
@@ -487,7 +510,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -495,14 +518,14 @@
         <v>1.74</v>
       </c>
       <c r="C7">
-        <f>((B7*0.001)/2)*13500</f>
+        <f t="shared" ref="C7:C15" si="0">((B7*0.001)/2)*13500</f>
         <v>11.744999999999999</v>
       </c>
       <c r="D7">
         <v>8.24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -510,14 +533,14 @@
         <v>1.76</v>
       </c>
       <c r="C8">
-        <f>((B8*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>11.88</v>
       </c>
       <c r="D8">
         <v>18.239999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -525,14 +548,14 @@
         <v>1.76</v>
       </c>
       <c r="C9">
-        <f>((B9*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>11.88</v>
       </c>
       <c r="D9">
         <v>28.24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -540,14 +563,14 @@
         <v>2.64</v>
       </c>
       <c r="C10">
-        <f>((B10*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>17.82</v>
       </c>
       <c r="D10">
         <v>10.74</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -555,14 +578,14 @@
         <v>2.68</v>
       </c>
       <c r="C11">
-        <f>((B11*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>18.09</v>
       </c>
       <c r="D11">
         <v>20.74</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -570,14 +593,14 @@
         <v>2.66</v>
       </c>
       <c r="C12">
-        <f>((B12*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>17.955000000000002</v>
       </c>
       <c r="D12">
         <v>30.74</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -585,14 +608,14 @@
         <v>3.52</v>
       </c>
       <c r="C13">
-        <f>((B13*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>23.76</v>
       </c>
       <c r="D13">
         <v>26.51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -600,14 +623,17 @@
         <v>3.52</v>
       </c>
       <c r="C14">
-        <f>((B14*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>23.76</v>
       </c>
       <c r="D14">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -615,19 +641,36 @@
         <v>3.52</v>
       </c>
       <c r="C15">
-        <f>((B15*0.001)/2)*13500</f>
+        <f t="shared" si="0"/>
         <v>23.76</v>
       </c>
       <c r="D15">
         <v>46.48</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(C4,C5,C6,C17,C18,C19,C30,C31,C32)</f>
+        <v>6.3405000000000014</v>
+      </c>
+      <c r="I16">
+        <f>_xlfn.STDEV.P(C4,C5,C6,C17,C19,C18,C30,C31,C32)</f>
+        <v>0.36458332380952374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -635,14 +678,25 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:C28" si="0">((B17*0.001)/2)*13500</f>
+        <f t="shared" ref="C17:C28" si="1">((B17*0.001)/2)*13500</f>
         <v>6.75</v>
       </c>
       <c r="D17">
         <v>36.979999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <f>AVERAGE(C7,C8,C9,C20,C21,C22,C33,C34,C35)</f>
+        <v>11.974499999999999</v>
+      </c>
+      <c r="I17">
+        <f>_xlfn.STDEV.P(C7,C8,C9,C20,C21,C22,C33,C34,C35)</f>
+        <v>0.16312112064352705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -650,14 +704,25 @@
         <v>1.02</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8850000000000007</v>
       </c>
       <c r="D18">
         <v>46.98</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f>AVERAGE(C38,C37,C36,C25,C24,C23,C12,C11,C10)</f>
+        <v>18.291000000000004</v>
+      </c>
+      <c r="I18">
+        <f>_xlfn.STDEV.P(C10,C11,C12,C23,C24,C25,C36,C37,C38)</f>
+        <v>0.24977589955798399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -665,14 +730,25 @@
         <v>1.016</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.8579999999999997</v>
       </c>
       <c r="D19">
         <v>56.96</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <f>AVERAGE(C13,C14,C15,C26,C27,C28,C39,C40,C41)</f>
+        <v>24.0825</v>
+      </c>
+      <c r="I19">
+        <f>_xlfn.STDEV.P(C15,C14,C13,C28,C27,C41,C40,C39,C26)</f>
+        <v>0.25411611519146116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -680,14 +756,14 @@
         <v>1.81</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.217500000000001</v>
       </c>
       <c r="D20">
         <v>37.24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -695,14 +771,14 @@
         <v>1.8</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.15</v>
       </c>
       <c r="D21">
         <v>47.24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -710,14 +786,14 @@
         <v>1.81</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.217500000000001</v>
       </c>
       <c r="D22">
         <v>57.25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -725,14 +801,14 @@
         <v>2.75</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.5625</v>
       </c>
       <c r="D23">
         <v>36.369999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -740,14 +816,14 @@
         <v>2.73</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.427500000000002</v>
       </c>
       <c r="D24">
         <v>46.46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -755,14 +831,14 @@
         <v>2.7280000000000002</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.414000000000001</v>
       </c>
       <c r="D25">
         <v>56.36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -770,14 +846,14 @@
         <v>3.56</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.03</v>
       </c>
       <c r="D26">
         <v>39.15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -785,14 +861,14 @@
         <v>3.62</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.435000000000002</v>
       </c>
       <c r="D27">
         <v>49.15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -800,19 +876,19 @@
         <v>3.61</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.3675</v>
       </c>
       <c r="D28">
         <v>59.15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -827,7 +903,7 @@
         <v>58.94</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -842,7 +918,7 @@
         <v>68.94</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -850,14 +926,14 @@
         <v>930</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32" si="1">((B32*0.000001)/2)*13500</f>
+        <f t="shared" ref="C32" si="2">((B32*0.000001)/2)*13500</f>
         <v>6.2774999999999999</v>
       </c>
       <c r="D32">
         <v>78.94</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -872,7 +948,7 @@
         <v>69.040000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -880,14 +956,14 @@
         <v>1.762</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:C41" si="2">((B34*0.001)/2)*13500</f>
+        <f t="shared" ref="C34:C41" si="3">((B34*0.001)/2)*13500</f>
         <v>11.893500000000001</v>
       </c>
       <c r="D34">
         <v>79.040000000000006</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -895,14 +971,14 @@
         <v>1.764</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.907</v>
       </c>
       <c r="D35">
         <v>89.04</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -910,14 +986,14 @@
         <v>2.74</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.495000000000001</v>
       </c>
       <c r="D36">
         <v>25.34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -925,14 +1001,14 @@
         <v>2.73</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.427500000000002</v>
       </c>
       <c r="D37">
         <v>35.24</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -940,14 +1016,14 @@
         <v>2.73</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.427500000000002</v>
       </c>
       <c r="D38">
         <v>45.24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -955,14 +1031,14 @@
         <v>3.58</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.165000000000003</v>
       </c>
       <c r="D39">
         <v>82.57</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -970,14 +1046,14 @@
         <v>3.58</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.165000000000003</v>
       </c>
       <c r="D40">
         <v>92.57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -985,7 +1061,7 @@
         <v>3.6</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.3</v>
       </c>
       <c r="D41">

</xml_diff>